<commit_message>
Add profile configuration and bug fix
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/06_Inst_Workspace.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/06_Inst_Workspace.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\src\app-catalog-main\installations-no-std\isp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dati\DEV\GitRepoAAAP\client-intesa\earlywarning-pom\earlywarning-config\src\baf-instances\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="3"/>
+    <workbookView xWindow="2040" yWindow="0" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Workspace" sheetId="1" r:id="rId1"/>
@@ -205,9 +205,6 @@
     <t>WS000000</t>
   </si>
   <si>
-    <t>Imprese Domestico</t>
-  </si>
-  <si>
     <t>CUSTOMER</t>
   </si>
   <si>
@@ -218,6 +215,9 @@
   </si>
   <si>
     <t>WS000000_TARGET</t>
+  </si>
+  <si>
+    <t>Corporate</t>
   </si>
 </sst>
 </file>
@@ -949,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,10 +996,10 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E3">
         <v>17</v>
@@ -1064,19 +1064,19 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
         <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1143,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,19 +1191,19 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
         <v>27</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>